<commit_message>
update water reservoir model
</commit_message>
<xml_diff>
--- a/Examples/ANP_Water_Reservoir/WaterReservior_Full_empty.xlsx
+++ b/Examples/ANP_Water_Reservoir/WaterReservior_Full_empty.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="14">
   <si>
     <t>1FloodControl</t>
   </si>
   <si>
-    <t>Enter judgments for the paiwise comparisons in the matrix or direct values in the green cells</t>
+    <t>Enter pairwise comparisons in the white cells of the table or numerical data in the green cells. For the Direct Values column, if the smallest value is best, invert the value before entering it (e.g., $10 as =1/10) .</t>
   </si>
   <si>
     <t>2Alternative Water Levels</t>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>3Hi</t>
+  </si>
+  <si>
+    <t>Line Sum</t>
+  </si>
+  <si>
+    <t>Estimated Priority</t>
+  </si>
+  <si>
+    <t>Sum of Col</t>
+  </si>
+  <si>
+    <t>Est. Incons.</t>
   </si>
   <si>
     <t>2Recreation</t>
@@ -50,7 +62,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +97,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +127,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFACCBE8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF6B"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -117,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9D5B6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,16 +183,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,17 +500,17 @@
     <col min="1" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -487,60 +526,120 @@
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9">
+        <f>+B4+C4+D4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <f>F4/F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="10">
         <f>1/C4</f>
         <v>0</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9">
+        <f>+B5+C5+D5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <f>F5/F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="10">
         <f>1/D4</f>
         <v>0</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="10">
         <f>1/D5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9">
+        <f>+B6+C6+D6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f>F6/F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="12">
+        <f>sum(B4:B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <f>sum(C4:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <f>sum(D4:D6)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <f>sum(F4:F6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="F8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="12">
+        <f>((MMULT(B7:D7,G4:G6)-3)/(3-1))/0.52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -556,60 +655,120 @@
       <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9">
+        <f>+B12+C12+D12</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <f>F12/F15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="10">
         <f>1/C12</f>
         <v>0</v>
       </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9">
+        <f>+B13+C13+D13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <f>F13/F15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="10">
         <f>1/D12</f>
         <v>0</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="10">
         <f>1/D13</f>
         <v>0</v>
       </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9">
+        <f>+B14+C14+D14</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <f>F14/F15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="12">
+        <f>sum(B12:B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="12">
+        <f>sum(C12:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="12">
+        <f>sum(D12:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <f>sum(F12:F14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="F16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="12">
+        <f>((MMULT(B15:D15,G12:G14)-3)/(3-1))/0.52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -625,255 +784,495 @@
       <c r="E19" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9">
+        <f>+B20+C20+D20</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <f>F20/F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="10">
         <f>1/C20</f>
         <v>0</v>
       </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9">
+        <f>+B21+C21+D21</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <f>F21/F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="10">
         <f>1/D20</f>
         <v>0</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="10">
         <f>1/D21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9">
+        <f>+B22+C22+D22</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <f>F22/F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="12">
+        <f>sum(B20:B22)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="12">
+        <f>sum(C20:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <f>sum(D20:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <f>sum(F20:F22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="F24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="12">
+        <f>((MMULT(B23:D23,G20:G22)-3)/(3-1))/0.52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9">
+        <f>+B28+C28+D28</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <f>F28/F31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="8">
+        <v>11</v>
+      </c>
+      <c r="B29" s="10">
         <f>1/C28</f>
         <v>0</v>
       </c>
-      <c r="C29" s="5">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="C29" s="6">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9">
+        <f>+B29+C29+D29</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <f>F29/F31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="8">
+        <v>12</v>
+      </c>
+      <c r="B30" s="10">
         <f>1/D28</f>
         <v>0</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="10">
         <f>1/D29</f>
         <v>0</v>
       </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9">
+        <f>+B30+C30+D30</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <f>F30/F31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="12">
+        <f>sum(B28:B30)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="12">
+        <f>sum(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="12">
+        <f>sum(D28:D30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <f>sum(F28:F30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="F32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="12">
+        <f>((MMULT(B31:D31,G28:G30)-3)/(3-1))/0.52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9">
+        <f>+B36+C36+D36</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <f>F36/F39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="8">
+        <v>11</v>
+      </c>
+      <c r="B37" s="10">
         <f>1/C36</f>
         <v>0</v>
       </c>
-      <c r="C37" s="5">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="9">
+        <f>+B37+C37+D37</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <f>F37/F39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="8">
+        <v>12</v>
+      </c>
+      <c r="B38" s="10">
         <f>1/D36</f>
         <v>0</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="10">
         <f>1/D37</f>
         <v>0</v>
       </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="9">
+        <f>+B38+C38+D38</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="9">
+        <f>F38/F39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="12">
+        <f>sum(B36:B38)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="12">
+        <f>sum(C36:C38)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="12">
+        <f>sum(D36:D38)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <f>sum(F36:F38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="F40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="12">
+        <f>((MMULT(B39:D39,G36:G38)-3)/(3-1))/0.52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:7">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:7">
       <c r="A43" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="5">
-        <v>1</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="B44" s="6">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="9">
+        <f>+B44+C44+D44</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="9">
+        <f>F44/F47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="8">
+        <v>11</v>
+      </c>
+      <c r="B45" s="10">
         <f>1/C44</f>
         <v>0</v>
       </c>
-      <c r="C45" s="5">
-        <v>1</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="C45" s="6">
+        <v>1</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9">
+        <f>+B45+C45+D45</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="9">
+        <f>F45/F47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="8">
+        <v>12</v>
+      </c>
+      <c r="B46" s="10">
         <f>1/D44</f>
         <v>0</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="10">
         <f>1/D45</f>
         <v>0</v>
       </c>
-      <c r="D46" s="5">
-        <v>1</v>
-      </c>
-      <c r="E46" s="7"/>
+      <c r="D46" s="6">
+        <v>1</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9">
+        <f>+B46+C46+D46</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="9">
+        <f>F46/F47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="12">
+        <f>sum(B44:B46)</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="12">
+        <f>sum(C44:C46)</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="12">
+        <f>sum(D44:D46)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="9">
+        <f>sum(F44:F46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="F48" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="12">
+        <f>((MMULT(B47:D47,G44:G46)-3)/(3-1))/0.52</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>